<commit_message>
Migrate railway management system to Spring Boot with REST APIs and H2 database.
Replit-Commit-Author: Agent
Replit-Commit-Session-Id: c667b704-1914-4146-992d-b6b88db80208
</commit_message>
<xml_diff>
--- a/data/passenger_tickets.xlsx
+++ b/data/passenger_tickets.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>S.No.</t>
   </si>
@@ -30,6 +30,27 @@
   </si>
   <si>
     <t>Seat Status</t>
+  </si>
+  <si>
+    <t>55555</t>
+  </si>
+  <si>
+    <t>Deep Mondal</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Confirmed</t>
+  </si>
+  <si>
+    <t>Qwe uiio</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>rttyy vvbbb</t>
   </si>
 </sst>
 </file>
@@ -74,7 +95,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -100,6 +121,66 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="D2" t="n" s="0">
+        <v>34.0</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="D3" t="n" s="0">
+        <v>78.0</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D4" t="n" s="0">
+        <v>98.0</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>